<commit_message>
Label was missing from the category
</commit_message>
<xml_diff>
--- a/brise_plandok/annotation/BRISE.xlsx
+++ b/brise_plandok/annotation/BRISE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\root\projects\brise-nlp\brise_nlp\annotation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\root\projects\brise-plandok\brise_plandok\annotation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A451BC7-75A3-4510-8586-C61D01FB975B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1D4A1F3-657E-41A6-A820-D51F4BBABEB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="46296" windowHeight="25536" xr2:uid="{4A4A6A95-EBA1-4E0C-8DC2-4A4B6AD8B4AB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
     <definedName name="NoAttribute">Label!$U$4</definedName>
     <definedName name="Nutzung_Widmung">Label!$M$4:$M$10</definedName>
     <definedName name="Stellplaetze_Garagen_Parkgebäude">Label!$I$4:$I$15</definedName>
-    <definedName name="Strassen_und_Gehsteige">Label!$R$4:$R$8</definedName>
+    <definedName name="Strassen_und_Gehsteige">Label!$R$4:$R$9</definedName>
     <definedName name="Volumen">Label!$F$4:$F$4</definedName>
     <definedName name="Vorbauten">Label!$K$4:$K$6</definedName>
   </definedNames>
@@ -839,7 +839,7 @@
   <dimension ref="A1:P346"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1308,8 +1308,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:U23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T4" sqref="T4:T9"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="I74" sqref="I74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Change Verkehrsflaeche_ID to VerkehrsflaecheID
</commit_message>
<xml_diff>
--- a/brise_plandok/annotation/BRISE.xlsx
+++ b/brise_plandok/annotation/BRISE.xlsx
@@ -375,7 +375,7 @@
     <t xml:space="preserve">DachneigungMin</t>
   </si>
   <si>
-    <t xml:space="preserve">Verkehrsflaeche_ID</t>
+    <t xml:space="preserve">VerkehrsflaecheID</t>
   </si>
   <si>
     <t xml:space="preserve">MaxHoeheWohngebaeude</t>
@@ -558,10 +558,10 @@
   <dimension ref="A1:P346"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="84.67"/>
@@ -1035,10 +1035,10 @@
   <dimension ref="B1:U23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P26" activeCellId="0" sqref="P26"/>
+      <selection pane="topLeft" activeCell="S12" activeCellId="0" sqref="S12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="56.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.55"/>

</xml_diff>

<commit_message>
Update labels in excel templates
</commit_message>
<xml_diff>
--- a/brise_plandok/annotation/BRISE.xlsx
+++ b/brise_plandok/annotation/BRISE.xlsx
@@ -26,7 +26,7 @@
     <definedName function="false" hidden="false" name="NoAttribute" vbProcedure="false">Label!$U$4</definedName>
     <definedName function="false" hidden="false" name="Nutzung_Widmung" vbProcedure="false">Label!$M$4:$M$10</definedName>
     <definedName function="false" hidden="false" name="Stellplaetze_Garagen_Parkgebäude" vbProcedure="false">Label!$I$4:$I$15</definedName>
-    <definedName function="false" hidden="false" name="Strassen_und_Gehsteige" vbProcedure="false">Label!$R$4:$R$9</definedName>
+    <definedName function="false" hidden="false" name="Strassen_und_Gehsteige" vbProcedure="false">Label!$R$4:$R$8</definedName>
     <definedName function="false" hidden="false" name="Volumen" vbProcedure="false">Label!$F$4:$F$4</definedName>
     <definedName function="false" hidden="false" name="Vorbauten" vbProcedure="false">Label!$K$4:$K$6</definedName>
   </definedNames>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="129">
   <si>
     <t xml:space="preserve">Sentence_ID</t>
   </si>
@@ -330,9 +330,6 @@
     <t xml:space="preserve">DachflaecheMin</t>
   </si>
   <si>
-    <t xml:space="preserve">VorkehrungBepflanzungOeffentlicheVerkehrsflaeche</t>
-  </si>
-  <si>
     <t xml:space="preserve">Planzeichen</t>
   </si>
   <si>
@@ -351,7 +348,7 @@
     <t xml:space="preserve">LaubengangHoehe</t>
   </si>
   <si>
-    <t xml:space="preserve">Bauweise_ID</t>
+    <t xml:space="preserve">BauweiseID</t>
   </si>
   <si>
     <t xml:space="preserve">DachneigungMax</t>
@@ -558,10 +555,10 @@
   <dimension ref="A1:P346"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="84.67"/>
@@ -1035,10 +1032,10 @@
   <dimension ref="B1:U23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S12" activeCellId="0" sqref="S12"/>
+      <selection pane="topLeft" activeCell="R34" activeCellId="0" sqref="R34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="56.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.55"/>
@@ -1366,14 +1363,11 @@
       <c r="Q9" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="R9" s="0" t="s">
+      <c r="S9" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="S9" s="0" t="s">
+      <c r="T9" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="T9" s="0" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1381,25 +1375,25 @@
         <v>24</v>
       </c>
       <c r="H10" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="I10" s="0" t="s">
         <v>99</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="M10" s="0" t="s">
         <v>100</v>
       </c>
-      <c r="M10" s="0" t="s">
+      <c r="O10" s="0" t="s">
         <v>101</v>
       </c>
-      <c r="O10" s="0" t="s">
+      <c r="P10" s="0" t="s">
         <v>102</v>
       </c>
-      <c r="P10" s="0" t="s">
+      <c r="Q10" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="Q10" s="0" t="s">
+      <c r="S10" s="0" t="s">
         <v>104</v>
-      </c>
-      <c r="S10" s="0" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1407,22 +1401,22 @@
         <v>25</v>
       </c>
       <c r="H11" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="I11" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="O11" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="O11" s="0" t="s">
+      <c r="P11" s="0" t="s">
         <v>108</v>
       </c>
-      <c r="P11" s="0" t="s">
+      <c r="Q11" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="Q11" s="0" t="s">
+      <c r="S11" s="0" t="s">
         <v>110</v>
-      </c>
-      <c r="S11" s="0" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1430,13 +1424,13 @@
         <v>19</v>
       </c>
       <c r="H12" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="I12" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="P12" s="0" t="s">
         <v>113</v>
-      </c>
-      <c r="P12" s="0" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1444,13 +1438,13 @@
         <v>16</v>
       </c>
       <c r="H13" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="I13" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="P13" s="0" t="s">
         <v>116</v>
-      </c>
-      <c r="P13" s="0" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1458,10 +1452,10 @@
         <v>22</v>
       </c>
       <c r="I14" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="P14" s="0" t="s">
         <v>118</v>
-      </c>
-      <c r="P14" s="0" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1469,10 +1463,10 @@
         <v>13</v>
       </c>
       <c r="I15" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="P15" s="0" t="s">
         <v>120</v>
-      </c>
-      <c r="P15" s="0" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1480,42 +1474,42 @@
         <v>18</v>
       </c>
       <c r="P16" s="0" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P17" s="0" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P18" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P19" s="0" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P20" s="0" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P21" s="0" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P22" s="0" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P23" s="0" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Delete Meta & NoAttri from templates
</commit_message>
<xml_diff>
--- a/brise_plandok/annotation/BRISE.xlsx
+++ b/brise_plandok/annotation/BRISE.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Label" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="Attribute" vbProcedure="false">Label!$B$1:$B$16</definedName>
+    <definedName function="false" hidden="false" name="Attribute" vbProcedure="false">Label!$B$1:$B$14</definedName>
     <definedName function="false" hidden="false" name="Ausgestaltung_und_Sonstiges" vbProcedure="false">Label!$P$4:$P$24</definedName>
     <definedName function="false" hidden="false" name="Dach" vbProcedure="false">Label!$Q$4:$Q$12</definedName>
     <definedName function="false" hidden="false" name="Einfriedungen" vbProcedure="false">Label!$L$4:$L$8</definedName>
@@ -22,8 +22,6 @@
     <definedName function="false" hidden="false" name="Hoehe" vbProcedure="false">Label!$H$4:$H$12</definedName>
     <definedName function="false" hidden="false" name="Lage_Gelaende_Planzeichen" vbProcedure="false">Label!$S$4:$S$11</definedName>
     <definedName function="false" hidden="false" name="Laubengaenge_Durchfahrten_Arkaden" vbProcedure="false">Label!$O$4:$O$11</definedName>
-    <definedName function="false" hidden="false" name="Meta" vbProcedure="false">Label!$T$4:$T$9</definedName>
-    <definedName function="false" hidden="false" name="NoAttribute" vbProcedure="false">Label!$U$4</definedName>
     <definedName function="false" hidden="false" name="Nutzung_Widmung" vbProcedure="false">Label!$M$4:$M$10</definedName>
     <definedName function="false" hidden="false" name="Stellplaetze_Garagen_Parkgebäude" vbProcedure="false">Label!$I$4:$I$15</definedName>
     <definedName function="false" hidden="false" name="Strassen_und_Gehsteige" vbProcedure="false">Label!$R$4:$R$8</definedName>
@@ -40,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="121">
   <si>
     <t xml:space="preserve">Sentence_ID</t>
   </si>
@@ -114,12 +112,6 @@
     <t xml:space="preserve">Lage_Gelaende_Planzeichen</t>
   </si>
   <si>
-    <t xml:space="preserve">Meta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NoAttribute</t>
-  </si>
-  <si>
     <t xml:space="preserve">VolumenUndUmbaubarerRaum</t>
   </si>
   <si>
@@ -162,9 +154,6 @@
     <t xml:space="preserve">AnFluchtlinie</t>
   </si>
   <si>
-    <t xml:space="preserve">AusnahmePruefungErforderlich</t>
-  </si>
-  <si>
     <t xml:space="preserve">BauklasseVIHoeheMax</t>
   </si>
   <si>
@@ -201,9 +190,6 @@
     <t xml:space="preserve">AnOeffentlichenVerkehrsflaechen</t>
   </si>
   <si>
-    <t xml:space="preserve">N/A</t>
-  </si>
-  <si>
     <t xml:space="preserve">BauklasseVIHoeheMin</t>
   </si>
   <si>
@@ -240,9 +226,6 @@
     <t xml:space="preserve">GelaendeneigungMin</t>
   </si>
   <si>
-    <t xml:space="preserve">Segmentierungsfehler</t>
-  </si>
-  <si>
     <t xml:space="preserve">FBOKMinimumWohnungen</t>
   </si>
   <si>
@@ -273,9 +256,6 @@
     <t xml:space="preserve">InSchutzzone</t>
   </si>
   <si>
-    <t xml:space="preserve">StrittigeBedeutung</t>
-  </si>
-  <si>
     <t xml:space="preserve">GebaeudeHoeheArt</t>
   </si>
   <si>
@@ -306,9 +286,6 @@
     <t xml:space="preserve">PlangebietAllgemein</t>
   </si>
   <si>
-    <t xml:space="preserve">WeitereBestimmungPruefungErforderlich</t>
-  </si>
-  <si>
     <t xml:space="preserve">GebaeudeHoeheMax</t>
   </si>
   <si>
@@ -331,9 +308,6 @@
   </si>
   <si>
     <t xml:space="preserve">Planzeichen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZuVorherigemSatzGehoerig</t>
   </si>
   <si>
     <t xml:space="preserve">GebaeudeHoeheMin</t>
@@ -558,7 +532,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="84.67"/>
@@ -1031,11 +1005,11 @@
   </sheetPr>
   <dimension ref="B1:U23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="O1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R34" activeCellId="0" sqref="R34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="56.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.55"/>
@@ -1068,7 +1042,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
@@ -1114,64 +1088,54 @@
       <c r="S3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="T3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="U3" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="I4" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="K4" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="L4" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="M4" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="L4" s="0" t="s">
+      <c r="N4" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="O4" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="P4" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="O4" s="0" t="s">
+      <c r="Q4" s="0" t="s">
         <v>35</v>
       </c>
-      <c r="P4" s="0" t="s">
+      <c r="R4" s="0" t="s">
         <v>36</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="S4" s="0" t="s">
         <v>37</v>
-      </c>
-      <c r="R4" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="S4" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="T4" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="U4" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1179,43 +1143,40 @@
         <v>17</v>
       </c>
       <c r="H5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5" s="0" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="0" t="s">
+      <c r="L5" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="J5" s="0" t="s">
+      <c r="M5" s="0" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="0" t="s">
+      <c r="N5" s="0" t="s">
         <v>44</v>
       </c>
-      <c r="L5" s="0" t="s">
+      <c r="O5" s="0" t="s">
         <v>45</v>
       </c>
-      <c r="M5" s="0" t="s">
+      <c r="P5" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="N5" s="0" t="s">
+      <c r="Q5" s="0" t="s">
         <v>47</v>
       </c>
-      <c r="O5" s="0" t="s">
+      <c r="R5" s="0" t="s">
         <v>48</v>
       </c>
-      <c r="P5" s="0" t="s">
+      <c r="S5" s="0" t="s">
         <v>49</v>
-      </c>
-      <c r="Q5" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="R5" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="S5" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="T5" s="0" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1223,43 +1184,40 @@
         <v>20</v>
       </c>
       <c r="H6" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="L6" s="0" t="s">
         <v>54</v>
       </c>
-      <c r="I6" s="0" t="s">
+      <c r="M6" s="0" t="s">
         <v>55</v>
       </c>
-      <c r="J6" s="0" t="s">
+      <c r="N6" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="K6" s="0" t="s">
+      <c r="O6" s="0" t="s">
         <v>57</v>
       </c>
-      <c r="L6" s="0" t="s">
+      <c r="P6" s="0" t="s">
         <v>58</v>
       </c>
-      <c r="M6" s="0" t="s">
+      <c r="Q6" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="N6" s="0" t="s">
+      <c r="R6" s="0" t="s">
         <v>60</v>
       </c>
-      <c r="O6" s="0" t="s">
+      <c r="S6" s="0" t="s">
         <v>61</v>
-      </c>
-      <c r="P6" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q6" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="R6" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="S6" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="T6" s="0" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1267,37 +1225,34 @@
         <v>15</v>
       </c>
       <c r="H7" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>65</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="O7" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="0" t="s">
+      <c r="P7" s="0" t="s">
         <v>68</v>
       </c>
-      <c r="J7" s="0" t="s">
+      <c r="Q7" s="0" t="s">
         <v>69</v>
       </c>
-      <c r="L7" s="0" t="s">
+      <c r="R7" s="0" t="s">
         <v>70</v>
       </c>
-      <c r="M7" s="0" t="s">
+      <c r="S7" s="0" t="s">
         <v>71</v>
-      </c>
-      <c r="O7" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="P7" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="Q7" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="R7" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="S7" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="T7" s="0" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1305,37 +1260,34 @@
         <v>23</v>
       </c>
       <c r="H8" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>73</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="L8" s="0" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="O8" s="0" t="s">
+        <v>77</v>
+      </c>
+      <c r="P8" s="0" t="s">
         <v>78</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="Q8" s="0" t="s">
         <v>79</v>
       </c>
-      <c r="J8" s="0" t="s">
+      <c r="R8" s="0" t="s">
         <v>80</v>
       </c>
-      <c r="L8" s="0" t="s">
+      <c r="S8" s="0" t="s">
         <v>81</v>
-      </c>
-      <c r="M8" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="O8" s="0" t="s">
-        <v>83</v>
-      </c>
-      <c r="P8" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q8" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="R8" s="0" t="s">
-        <v>86</v>
-      </c>
-      <c r="S8" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="T8" s="0" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1343,173 +1295,164 @@
         <v>21</v>
       </c>
       <c r="H9" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="M9" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="O9" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q9" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="S9" s="0" t="s">
         <v>89</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="M9" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="O9" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="P9" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q9" s="0" t="s">
-        <v>95</v>
-      </c>
-      <c r="S9" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="T9" s="0" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="S10" s="0" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="S11" s="0" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="P12" s="0" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="P13" s="0" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="P14" s="0" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="5" t="s">
-        <v>13</v>
-      </c>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I15" s="0" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="P15" s="0" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="5" t="s">
-        <v>18</v>
-      </c>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P16" s="0" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P17" s="0" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P18" s="0" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P19" s="0" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P20" s="0" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P21" s="0" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P22" s="0" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P23" s="0" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add EinleitungNiederschlagswaesser to excel templates
</commit_message>
<xml_diff>
--- a/brise_plandok/annotation/BRISE.xlsx
+++ b/brise_plandok/annotation/BRISE.xlsx
@@ -13,7 +13,7 @@
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" name="Attribute" vbProcedure="false">Label!$B$1:$B$14</definedName>
-    <definedName function="false" hidden="false" name="Ausgestaltung_und_Sonstiges" vbProcedure="false">Label!$P$4:$P$23</definedName>
+    <definedName function="false" hidden="false" name="Ausgestaltung_und_Sonstiges" vbProcedure="false">Label!$P$4:$P$24</definedName>
     <definedName function="false" hidden="false" name="Dach" vbProcedure="false">Label!$Q$4:$Q$12</definedName>
     <definedName function="false" hidden="false" name="Einfriedungen" vbProcedure="false">Label!$L$4:$L$8</definedName>
     <definedName function="false" hidden="false" name="Flaeche" vbProcedure="false">Label!$G$4:$G$4</definedName>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="123">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -367,16 +367,19 @@
     <t xml:space="preserve">StellplatzregulativVorhanden</t>
   </si>
   <si>
+    <t xml:space="preserve">EinleitungNiederschlagswaesser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">StellplatzverpflichtungArt</t>
+  </si>
+  <si>
     <t xml:space="preserve">ErrichtungGebaeude</t>
   </si>
   <si>
-    <t xml:space="preserve">StellplatzverpflichtungArt</t>
+    <t xml:space="preserve">VerbotStellplaetzeUndParkgebaeude</t>
   </si>
   <si>
     <t xml:space="preserve">GebaeudeBautyp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VerbotStellplaetzeUndParkgebaeude</t>
   </si>
   <si>
     <t xml:space="preserve">Kleinhaeuser</t>
@@ -596,7 +599,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="57.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -731,13 +734,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:U23"/>
+  <dimension ref="B1:U24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="O23" activeCellId="0" sqref="O23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="56.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.55"/>
@@ -1148,39 +1151,44 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P17" s="0" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P18" s="0" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P19" s="0" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P20" s="0" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P21" s="0" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P22" s="0" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="P23" s="0" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P24" s="0" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>